<commit_message>
Toma de datos de iPoint terminada
</commit_message>
<xml_diff>
--- a/src/proyecto/SKU_Integrar.xlsx
+++ b/src/proyecto/SKU_Integrar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mis_entornos\minderest\src\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DC56D8-C85F-4362-A542-415092689D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B55B0D-E195-439B-9626-0FDDDC1F564D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,10 @@
     <t>SKU</t>
   </si>
   <si>
-    <t>PRUEBA2</t>
+    <t>SWSUOP101</t>
   </si>
   <si>
-    <t>kit-gm00002</t>
+    <t>SWSUOP400</t>
   </si>
 </sst>
 </file>
@@ -354,10 +354,13 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -366,12 +369,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>